<commit_message>
Corrected grammatical errors. Fixed functionality for larger images. Current state is believed to be complete.
</commit_message>
<xml_diff>
--- a/Test Metrics.xlsx
+++ b/Test Metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chukl\OneDrive\Documents\UniOfLincoln\Parallel Programming\CMP3752M-Assessment-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D6C53BF-0DE1-4612-A0F8-9CC232AB2944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7F8580-C588-4DF5-804D-48E2200712CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{58ABF0F4-5306-42C2-89B5-229A25C20A15}"/>
+    <workbookView xWindow="-26460" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{58ABF0F4-5306-42C2-89B5-229A25C20A15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Test 1</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>8-bit</t>
+  </si>
+  <si>
+    <t>test.pgm</t>
+  </si>
+  <si>
+    <t>test_large.pgm</t>
   </si>
 </sst>
 </file>
@@ -456,15 +462,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588FD223-CF4C-491C-8A19-0F8A4282FDBC}">
-  <dimension ref="A2:G18"/>
+  <dimension ref="A2:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="B20" sqref="B20:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -775,6 +781,54 @@
         <v>55352281.600000001</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>1228800</v>
+      </c>
+      <c r="C20">
+        <v>1230848</v>
+      </c>
+      <c r="D20">
+        <v>1163232</v>
+      </c>
+      <c r="E20">
+        <v>1361920</v>
+      </c>
+      <c r="F20">
+        <v>1156096</v>
+      </c>
+      <c r="G20" s="1">
+        <f t="shared" ref="G20:G21" si="3">AVERAGE(B20:F20)</f>
+        <v>1228179.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>22693696</v>
+      </c>
+      <c r="C21">
+        <v>24498176</v>
+      </c>
+      <c r="D21">
+        <v>24958976</v>
+      </c>
+      <c r="E21">
+        <v>26193920</v>
+      </c>
+      <c r="F21">
+        <v>26352480</v>
+      </c>
+      <c r="G21" s="1">
+        <f t="shared" si="3"/>
+        <v>24939449.600000001</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>